<commit_message>
made the functions as per testcase document
</commit_message>
<xml_diff>
--- a/testdata/testData.xlsx
+++ b/testdata/testData.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="44">
   <si>
     <t>windows authentication</t>
   </si>
@@ -121,6 +121,36 @@
   </si>
   <si>
     <t>create case in sandy</t>
+  </si>
+  <si>
+    <t>Smarter Quoting</t>
+  </si>
+  <si>
+    <t>kathmandu\yamah022</t>
+  </si>
+  <si>
+    <t>10.0.1.62:70</t>
+  </si>
+  <si>
+    <t>10.0.1.62:71</t>
+  </si>
+  <si>
+    <t>10.0.1.62:72</t>
+  </si>
+  <si>
+    <t>10.0.1.62:75</t>
+  </si>
+  <si>
+    <t>10.0.1.62:90</t>
+  </si>
+  <si>
+    <t>10.0.1.62:91</t>
+  </si>
+  <si>
+    <t>10.0.1.62:92</t>
+  </si>
+  <si>
+    <t>10.0.1.62:94</t>
   </si>
 </sst>
 </file>
@@ -188,7 +218,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -196,15 +226,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -486,76 +520,94 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="20.88671875" style="2" customWidth="1"/>
     <col min="2" max="2" width="24" style="2" customWidth="1"/>
-    <col min="3" max="3" width="14.88671875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="14.109375" style="2" customWidth="1"/>
-    <col min="5" max="5" width="14" style="2" customWidth="1"/>
+    <col min="3" max="3" width="18.77734375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="20.33203125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="18.6640625" style="2" customWidth="1"/>
     <col min="6" max="6" width="11.33203125" style="2" customWidth="1"/>
-    <col min="7" max="16384" width="8.88671875" style="2"/>
+    <col min="7" max="7" width="8.88671875" style="2"/>
+    <col min="8" max="8" width="19.88671875" style="2" customWidth="1"/>
+    <col min="9" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="D1" s="3" t="s">
+      <c r="B1" s="5"/>
+      <c r="D1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="3"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
+      <c r="E1" s="5"/>
+      <c r="G1" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="H1" s="5"/>
+    </row>
+    <row r="2" spans="1:8" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="4"/>
-      <c r="D2" s="4" t="s">
+      <c r="B2" s="3"/>
+      <c r="D2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
+      <c r="G2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="4"/>
-      <c r="D3" s="4" t="s">
+      <c r="B3" s="3"/>
+      <c r="D3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="4" t="s">
+      <c r="G3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="4"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="s">
+      <c r="B4" s="3"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="4"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="4" t="s">
+      <c r="B5" s="3"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="4"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B6" s="3"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B10" s="1" t="s">
         <v>13</v>
       </c>
@@ -572,119 +624,142 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D11" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="E11" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="F11" s="4" t="s">
+      <c r="F11" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4" t="s">
+      <c r="B12" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="F12" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>23</v>
       </c>
+      <c r="B15" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F15" s="3"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" s="3" t="s">
+      <c r="A17" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B17" s="3"/>
+      <c r="B17" s="5"/>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" s="1" t="s">
+      <c r="A18" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="3" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" s="1" t="s">
+      <c r="A19" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B19" s="2">
+      <c r="B19" s="3">
         <v>587</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" s="1" t="s">
+      <c r="A20" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="3" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21" s="1" t="s">
+      <c r="A21" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B21" s="3" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A22" s="1" t="s">
+      <c r="A22" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="7" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A23" s="1" t="s">
+      <c r="A23" s="6" t="s">
         <v>33</v>
       </c>
+      <c r="B23" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="A17:B17"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="D1:E1"/>
+    <mergeCell ref="G1:H1"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E3" r:id="rId1"/>

</xml_diff>